<commit_message>
add multi compare audio and payload
</commit_message>
<xml_diff>
--- a/quality_result.xlsx
+++ b/quality_result.xlsx
@@ -524,19 +524,19 @@
         <v>0.09448330857870649</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1139771048046652</v>
+        <v>0.1139317528165474</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1323182046659637</v>
+        <v>0.1323295426629932</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1498996587262894</v>
+        <v>0.1499336727173778</v>
       </c>
       <c r="K2" t="n">
-        <v>0.16887946575358</v>
+        <v>0.168830334433119</v>
       </c>
       <c r="L2" t="n">
-        <v>0.178565894549069</v>
+        <v>0.1786301431989025</v>
       </c>
     </row>
     <row r="3">
@@ -546,37 +546,37 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.001844314183456351</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01911964232398704</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.03781977875788464</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.05630071391587962</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.07593812477087798</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.09448330857870649</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1139317528165474</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1277225365366954</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1236144022796933</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1394195701387393</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0.1529873732506415</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -586,37 +586,37 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.001855652180485795</v>
+        <v>0.003870036319383817</v>
       </c>
       <c r="C4" t="n">
-        <v>0.01911964232398704</v>
+        <v>0.03722642358001035</v>
       </c>
       <c r="D4" t="n">
-        <v>0.03781977875788464</v>
+        <v>0.07481188373261979</v>
       </c>
       <c r="E4" t="n">
-        <v>0.05630071391587962</v>
+        <v>0.1125938691670729</v>
       </c>
       <c r="F4" t="n">
-        <v>0.07593812477087798</v>
+        <v>0.1502775919606043</v>
       </c>
       <c r="G4" t="n">
-        <v>0.09448330857870649</v>
+        <v>0.1887322985521378</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1139317528165474</v>
+        <v>0.2241673186014959</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1323182046659637</v>
+        <v>0.2608230629976908</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1500810666787605</v>
+        <v>0.3005325079271496</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1704478886759865</v>
+        <v>0.3344633537039347</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1890799971277074</v>
+        <v>0.373167496230116</v>
       </c>
     </row>
     <row r="5">
@@ -632,13 +632,13 @@
         <v>0.01911964232398704</v>
       </c>
       <c r="D5" t="n">
-        <v>0.03783111675491407</v>
+        <v>0.03781977875788464</v>
       </c>
       <c r="E5" t="n">
-        <v>0.05631205191290906</v>
+        <v>0.05630071391587962</v>
       </c>
       <c r="F5" t="n">
-        <v>0.07594946276790743</v>
+        <v>0.07593812477087798</v>
       </c>
       <c r="G5" t="n">
         <v>0.09448330857870649</v>
@@ -650,13 +650,13 @@
         <v>0.1323295426629932</v>
       </c>
       <c r="J5" t="n">
-        <v>0.1499223347203483</v>
+        <v>0.15009240467579</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1686262504865891</v>
+        <v>0.1686375884836185</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1793633336734732</v>
+        <v>0.1792612917002082</v>
       </c>
     </row>
     <row r="6">
@@ -666,37 +666,37 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.001844314183456351</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01911964232398704</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.03781977875788464</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.05630071391587962</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.07593812477087798</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.09448330857870649</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1139317528165474</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0.1323182046659637</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>0.1500810666787605</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.163629973128947</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>0.154325256900116</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -709,7 +709,7 @@
         <v>0.001844314183456351</v>
       </c>
       <c r="C7" t="n">
-        <v>0.01911964232398704</v>
+        <v>0.01913098032101649</v>
       </c>
       <c r="D7" t="n">
         <v>0.03781977875788464</v>
@@ -727,16 +727,16 @@
         <v>0.1139317528165474</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1323182046659637</v>
+        <v>0.1322917493395617</v>
       </c>
       <c r="J7" t="n">
         <v>0.1497598234295929</v>
       </c>
       <c r="K7" t="n">
-        <v>0.1655309772975506</v>
+        <v>0.1654364939889719</v>
       </c>
       <c r="L7" t="n">
-        <v>0.1677305487212629</v>
+        <v>0.1675340234394192</v>
       </c>
     </row>
     <row r="8">
@@ -749,7 +749,7 @@
         <v>0.001855652180485795</v>
       </c>
       <c r="C8" t="n">
-        <v>0.01911964232398704</v>
+        <v>0.01913098032101649</v>
       </c>
       <c r="D8" t="n">
         <v>0.03781977875788464</v>
@@ -770,13 +770,13 @@
         <v>0.1323182046659637</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1462526030151513</v>
+        <v>0.1463584243207595</v>
       </c>
       <c r="K8" t="n">
-        <v>0.1651190300721475</v>
+        <v>0.1651870580543241</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1710601405155765</v>
+        <v>0.1708825118954486</v>
       </c>
     </row>
     <row r="9">
@@ -813,10 +813,10 @@
         <v>0.1500810666787605</v>
       </c>
       <c r="K9" t="n">
-        <v>0.1658068685586004</v>
+        <v>0.1660033938404442</v>
       </c>
       <c r="L9" t="n">
-        <v>0.1678741633503025</v>
+        <v>0.1677985767034396</v>
       </c>
     </row>
     <row r="10">
@@ -838,25 +838,25 @@
         <v>0.05630071391587962</v>
       </c>
       <c r="F10" t="n">
-        <v>0.07593812477087798</v>
+        <v>0.07594946276790743</v>
       </c>
       <c r="G10" t="n">
-        <v>0.09448330857870649</v>
+        <v>16231.70793319652</v>
       </c>
       <c r="H10" t="n">
-        <v>16231.72738164076</v>
+        <v>0.1139430908135769</v>
       </c>
       <c r="I10" t="n">
-        <v>16231.74576809261</v>
+        <v>0.1323182046659637</v>
       </c>
       <c r="J10" t="n">
-        <v>0.15009240467579</v>
+        <v>0.1501037426728194</v>
       </c>
       <c r="K10" t="n">
-        <v>0.169722256866102</v>
+        <v>16231.78326662812</v>
       </c>
       <c r="L10" t="n">
-        <v>0.1821222462839715</v>
+        <v>16231.7956741762</v>
       </c>
     </row>
     <row r="11">
@@ -896,7 +896,7 @@
         <v>0.1704478886759865</v>
       </c>
       <c r="L11" t="n">
-        <v>0.1803459600826918</v>
+        <v>0.1802514767741131</v>
       </c>
     </row>
     <row r="12">
@@ -927,16 +927,16 @@
         <v>0.1139430908135769</v>
       </c>
       <c r="I12" t="n">
-        <v>0.131154170304274</v>
+        <v>0.1323295426629932</v>
       </c>
       <c r="J12" t="n">
-        <v>0.1356326791309047</v>
+        <v>0.1500810666787605</v>
       </c>
       <c r="K12" t="n">
-        <v>0.1537923710397321</v>
+        <v>0.1540418069743799</v>
       </c>
       <c r="L12" t="n">
-        <v>0.1386410276760507</v>
+        <v>0.1384482817265502</v>
       </c>
     </row>
     <row r="13">
@@ -973,10 +973,10 @@
         <v>0.1500810666787605</v>
       </c>
       <c r="K13" t="n">
-        <v>0.1697184775337589</v>
+        <v>0.1697109188690726</v>
       </c>
       <c r="L13" t="n">
-        <v>0.1825644281681198</v>
+        <v>0.1824964001859432</v>
       </c>
     </row>
     <row r="14">
@@ -1007,16 +1007,16 @@
         <v>0.1139317528165474</v>
       </c>
       <c r="I14" t="n">
-        <v>0.1287542942663749</v>
+        <v>0.1320687687313159</v>
       </c>
       <c r="J14" t="n">
-        <v>0.1420424267848842</v>
+        <v>0.1420348681201979</v>
       </c>
       <c r="K14" t="n">
-        <v>0.142930569885524</v>
+        <v>0.1434521177488785</v>
       </c>
       <c r="L14" t="n">
-        <v>0.1552134000007559</v>
+        <v>0.1558407691697185</v>
       </c>
     </row>
     <row r="15">
@@ -1056,7 +1056,7 @@
         <v>0.1704478886759865</v>
       </c>
       <c r="L15" t="n">
-        <v>0.1853951480931379</v>
+        <v>0.1855425420545206</v>
       </c>
     </row>
     <row r="16">
@@ -1093,10 +1093,10 @@
         <v>0.1500810666787605</v>
       </c>
       <c r="K16" t="n">
-        <v>0.1696542288839254</v>
+        <v>0.1705499306492515</v>
       </c>
       <c r="L16" t="n">
-        <v>0.1832900599780043</v>
+        <v>0.1833769846218967</v>
       </c>
     </row>
   </sheetData>
@@ -1200,19 +1200,19 @@
         <v>100.6693752668236</v>
       </c>
       <c r="H2" t="n">
-        <v>99.85474998480416</v>
+        <v>99.85647840542357</v>
       </c>
       <c r="I2" t="n">
-        <v>99.20673019897004</v>
+        <v>99.20635807945658</v>
       </c>
       <c r="J2" t="n">
-        <v>98.66491975405155</v>
+        <v>98.66393440071346</v>
       </c>
       <c r="K2" t="n">
-        <v>98.14715773083675</v>
+        <v>98.14842138747352</v>
       </c>
       <c r="L2" t="n">
-        <v>97.90494105733396</v>
+        <v>97.90337873124719</v>
       </c>
     </row>
     <row r="3">
@@ -1221,38 +1221,60 @@
           <t>Audio2</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>117.6618425981262</v>
-      </c>
-      <c r="C3" t="n">
-        <v>107.5053940240677</v>
-      </c>
-      <c r="D3" t="n">
-        <v>104.5430018203052</v>
-      </c>
-      <c r="E3" t="n">
-        <v>102.815052640491</v>
-      </c>
-      <c r="F3" t="n">
-        <v>101.5155929757197</v>
-      </c>
-      <c r="G3" t="n">
-        <v>100.566640731433</v>
-      </c>
-      <c r="H3" t="n">
-        <v>99.75374387003292</v>
-      </c>
-      <c r="I3" t="n">
-        <v>99.25751631035821</v>
-      </c>
-      <c r="J3" t="n">
-        <v>99.39950092735265</v>
-      </c>
-      <c r="K3" t="n">
-        <v>98.8769542658853</v>
-      </c>
-      <c r="L3" t="n">
-        <v>98.47363577983592</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -1262,37 +1284,37 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>117.9301018750046</v>
+        <v>114.7379172298362</v>
       </c>
       <c r="C4" t="n">
-        <v>107.8002700021487</v>
+        <v>104.9065544912582</v>
       </c>
       <c r="D4" t="n">
-        <v>104.8378777983862</v>
+        <v>101.8753617353521</v>
       </c>
       <c r="E4" t="n">
-        <v>103.109928618572</v>
+        <v>100.0999202032218</v>
       </c>
       <c r="F4" t="n">
-        <v>101.8104689538007</v>
+        <v>98.84612536436006</v>
       </c>
       <c r="G4" t="n">
-        <v>100.8615167095139</v>
+        <v>97.85660534606841</v>
       </c>
       <c r="H4" t="n">
-        <v>100.0486198481139</v>
+        <v>97.10934466779599</v>
       </c>
       <c r="I4" t="n">
-        <v>99.39887164166038</v>
+        <v>96.4516077299519</v>
       </c>
       <c r="J4" t="n">
-        <v>98.85180856044472</v>
+        <v>95.83615308234175</v>
       </c>
       <c r="K4" t="n">
-        <v>98.29915137745472</v>
+        <v>95.3715822360107</v>
       </c>
       <c r="L4" t="n">
-        <v>97.84861176740023</v>
+        <v>94.89602955126401</v>
       </c>
     </row>
     <row r="5">
@@ -1308,13 +1330,13 @@
         <v>107.5429037904572</v>
       </c>
       <c r="D5" t="n">
-        <v>104.5792098097497</v>
+        <v>104.5805115866948</v>
       </c>
       <c r="E5" t="n">
-        <v>102.8516879004201</v>
+        <v>102.8525624068806</v>
       </c>
       <c r="F5" t="n">
-        <v>101.5524543639719</v>
+        <v>101.5531027421092</v>
       </c>
       <c r="G5" t="n">
         <v>100.6041504978225</v>
@@ -1326,13 +1348,13 @@
         <v>99.14113331045547</v>
       </c>
       <c r="J5" t="n">
-        <v>98.59903805798535</v>
+        <v>98.5941142698244</v>
       </c>
       <c r="K5" t="n">
-        <v>98.08844959302319</v>
+        <v>98.08815759435753</v>
       </c>
       <c r="L5" t="n">
-        <v>97.8203647541699</v>
+        <v>97.82283621117379</v>
       </c>
     </row>
     <row r="6">
@@ -1341,38 +1363,60 @@
           <t>Audio5</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>117.6620392446475</v>
-      </c>
-      <c r="C6" t="n">
-        <v>107.5055906705889</v>
-      </c>
-      <c r="D6" t="n">
-        <v>104.5431984668265</v>
-      </c>
-      <c r="E6" t="n">
-        <v>102.8152492870123</v>
-      </c>
-      <c r="F6" t="n">
-        <v>101.515789622241</v>
-      </c>
-      <c r="G6" t="n">
-        <v>100.5668373779542</v>
-      </c>
-      <c r="H6" t="n">
-        <v>99.7539405165542</v>
-      </c>
-      <c r="I6" t="n">
-        <v>99.10419231010067</v>
-      </c>
-      <c r="J6" t="n">
-        <v>98.55712922888503</v>
-      </c>
-      <c r="K6" t="n">
-        <v>98.18175971549933</v>
-      </c>
-      <c r="L6" t="n">
-        <v>98.436018220223</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -1385,7 +1429,7 @@
         <v>117.6973335758085</v>
       </c>
       <c r="C7" t="n">
-        <v>107.5408850017499</v>
+        <v>107.5383103876132</v>
       </c>
       <c r="D7" t="n">
         <v>104.5784927979875</v>
@@ -1403,16 +1447,16 @@
         <v>99.78923484771516</v>
       </c>
       <c r="I7" t="n">
-        <v>99.13948664126164</v>
+        <v>99.14035504414201</v>
       </c>
       <c r="J7" t="n">
         <v>98.60172944382937</v>
       </c>
       <c r="K7" t="n">
-        <v>98.16688984591779</v>
+        <v>98.16936946003231</v>
       </c>
       <c r="L7" t="n">
-        <v>98.10956095982544</v>
+        <v>98.11465245247463</v>
       </c>
     </row>
     <row r="8">
@@ -1425,7 +1469,7 @@
         <v>117.6666863050063</v>
       </c>
       <c r="C8" t="n">
-        <v>107.5368544321503</v>
+        <v>107.5342798180136</v>
       </c>
       <c r="D8" t="n">
         <v>104.5744622283878</v>
@@ -1446,13 +1490,13 @@
         <v>99.13545607166201</v>
       </c>
       <c r="J8" t="n">
-        <v>98.70061602343927</v>
+        <v>98.69747481502239</v>
       </c>
       <c r="K8" t="n">
-        <v>98.17368077914026</v>
+        <v>98.17189188218958</v>
       </c>
       <c r="L8" t="n">
-        <v>98.02016382333801</v>
+        <v>98.02467587446381</v>
       </c>
     </row>
     <row r="9">
@@ -1489,10 +1533,10 @@
         <v>98.51907464438975</v>
       </c>
       <c r="K9" t="n">
-        <v>98.08630854908515</v>
+        <v>98.08116405145434</v>
       </c>
       <c r="L9" t="n">
-        <v>98.03249510918725</v>
+        <v>98.03445099420715</v>
       </c>
     </row>
     <row r="10">
@@ -1514,25 +1558,25 @@
         <v>103.0331359461823</v>
       </c>
       <c r="F10" t="n">
-        <v>101.733676281411</v>
+        <v>101.7330279032736</v>
       </c>
       <c r="G10" t="n">
-        <v>100.7847240371242</v>
+        <v>48.43463276958698</v>
       </c>
       <c r="H10" t="n">
-        <v>48.43462756597749</v>
+        <v>99.97139500607605</v>
       </c>
       <c r="I10" t="n">
-        <v>48.43462264651953</v>
+        <v>99.32207896927066</v>
       </c>
       <c r="J10" t="n">
-        <v>98.77468780912615</v>
+        <v>98.77435975497946</v>
       </c>
       <c r="K10" t="n">
-        <v>98.24088698410705</v>
+        <v>48.43461261347164</v>
       </c>
       <c r="L10" t="n">
-        <v>97.93464498305457</v>
+        <v>48.43460929373313</v>
       </c>
     </row>
     <row r="11">
@@ -1572,7 +1616,7 @@
         <v>98.0252437107056</v>
       </c>
       <c r="L11" t="n">
-        <v>97.78009578935807</v>
+        <v>97.78237165581149</v>
       </c>
     </row>
     <row r="12">
@@ -1603,16 +1647,16 @@
         <v>99.74887814202577</v>
       </c>
       <c r="I12" t="n">
-        <v>99.13793705738178</v>
+        <v>99.09918998570696</v>
       </c>
       <c r="J12" t="n">
-        <v>98.99211469740543</v>
+        <v>98.55249902400476</v>
       </c>
       <c r="K12" t="n">
-        <v>98.44641017560939</v>
+        <v>98.43937205694347</v>
       </c>
       <c r="L12" t="n">
-        <v>98.89684041205723</v>
+        <v>98.90288240017716</v>
       </c>
     </row>
     <row r="13">
@@ -1649,10 +1693,10 @@
         <v>98.61142798344098</v>
       </c>
       <c r="K13" t="n">
-        <v>98.07739578816791</v>
+        <v>98.07758921197852</v>
       </c>
       <c r="L13" t="n">
-        <v>97.76052544897095</v>
+        <v>97.76214403827561</v>
       </c>
     </row>
     <row r="14">
@@ -1683,16 +1727,16 @@
         <v>99.74420341108315</v>
       </c>
       <c r="I14" t="n">
-        <v>99.21303397346875</v>
+        <v>99.10264991110512</v>
       </c>
       <c r="J14" t="n">
-        <v>98.78647036486826</v>
+        <v>98.78670147706367</v>
       </c>
       <c r="K14" t="n">
-        <v>98.75939994759395</v>
+        <v>98.74358156056888</v>
       </c>
       <c r="L14" t="n">
-        <v>98.40135907689769</v>
+        <v>98.38384037021207</v>
       </c>
     </row>
     <row r="15">
@@ -1732,7 +1776,7 @@
         <v>98.15598711522031</v>
       </c>
       <c r="L15" t="n">
-        <v>97.79091973350884</v>
+        <v>97.78746835128679</v>
       </c>
     </row>
     <row r="16">
@@ -1769,10 +1813,10 @@
         <v>98.62074222478994</v>
       </c>
       <c r="K16" t="n">
-        <v>98.08835440656298</v>
+        <v>98.06548583061891</v>
       </c>
       <c r="L16" t="n">
-        <v>97.75261216875757</v>
+        <v>97.75055303121319</v>
       </c>
     </row>
   </sheetData>
@@ -1876,19 +1920,19 @@
         <v>106.5759151470831</v>
       </c>
       <c r="H2" t="n">
-        <v>105.7612898650637</v>
+        <v>105.7630182856831</v>
       </c>
       <c r="I2" t="n">
-        <v>105.1132700792296</v>
+        <v>105.1128979597161</v>
       </c>
       <c r="J2" t="n">
-        <v>104.571459634311</v>
+        <v>104.570474280973</v>
       </c>
       <c r="K2" t="n">
-        <v>104.0536976110962</v>
+        <v>104.054961267733</v>
       </c>
       <c r="L2" t="n">
-        <v>103.8114809375934</v>
+        <v>103.8099186115067</v>
       </c>
     </row>
     <row r="3">
@@ -1897,38 +1941,60 @@
           <t>Audio2</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>123.6711170137764</v>
-      </c>
-      <c r="C3" t="n">
-        <v>113.5146684397178</v>
-      </c>
-      <c r="D3" t="n">
-        <v>110.5522762359554</v>
-      </c>
-      <c r="E3" t="n">
-        <v>108.8243270561412</v>
-      </c>
-      <c r="F3" t="n">
-        <v>107.5248673913698</v>
-      </c>
-      <c r="G3" t="n">
-        <v>106.5759151470831</v>
-      </c>
-      <c r="H3" t="n">
-        <v>105.7630182856831</v>
-      </c>
-      <c r="I3" t="n">
-        <v>105.2667907260084</v>
-      </c>
-      <c r="J3" t="n">
-        <v>105.4087753430028</v>
-      </c>
-      <c r="K3" t="n">
-        <v>104.8862286815355</v>
-      </c>
-      <c r="L3" t="n">
-        <v>104.4829101954861</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -1938,37 +2004,37 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>123.6445003125738</v>
+        <v>120.4523156674054</v>
       </c>
       <c r="C4" t="n">
-        <v>113.5146684397178</v>
+        <v>110.6209529288274</v>
       </c>
       <c r="D4" t="n">
-        <v>110.5522762359554</v>
+        <v>107.5897601729213</v>
       </c>
       <c r="E4" t="n">
-        <v>108.8243270561412</v>
+        <v>105.814318640791</v>
       </c>
       <c r="F4" t="n">
-        <v>107.5248673913698</v>
+        <v>104.5605238019292</v>
       </c>
       <c r="G4" t="n">
-        <v>106.5759151470831</v>
+        <v>103.5710037836376</v>
       </c>
       <c r="H4" t="n">
-        <v>105.7630182856831</v>
+        <v>102.8237431053652</v>
       </c>
       <c r="I4" t="n">
-        <v>105.1132700792296</v>
+        <v>102.166006167521</v>
       </c>
       <c r="J4" t="n">
-        <v>104.5662069980139</v>
+        <v>101.5505515199109</v>
       </c>
       <c r="K4" t="n">
-        <v>104.0135498150239</v>
+        <v>101.0859806735799</v>
       </c>
       <c r="L4" t="n">
-        <v>103.5630102049694</v>
+        <v>100.6104279888332</v>
       </c>
     </row>
     <row r="5">
@@ -1984,13 +2050,13 @@
         <v>113.5146684397178</v>
       </c>
       <c r="D5" t="n">
-        <v>110.5509744590103</v>
+        <v>110.5522762359554</v>
       </c>
       <c r="E5" t="n">
-        <v>108.8234525496808</v>
+        <v>108.8243270561412</v>
       </c>
       <c r="F5" t="n">
-        <v>107.5242190132325</v>
+        <v>107.5248673913698</v>
       </c>
       <c r="G5" t="n">
         <v>106.5759151470831</v>
@@ -2002,13 +2068,13 @@
         <v>105.1128979597161</v>
       </c>
       <c r="J5" t="n">
-        <v>104.570802707246</v>
+        <v>104.565878919085</v>
       </c>
       <c r="K5" t="n">
-        <v>104.0602142422838</v>
+        <v>104.0599222436181</v>
       </c>
       <c r="L5" t="n">
-        <v>103.7921294034305</v>
+        <v>103.7946008604344</v>
       </c>
     </row>
     <row r="6">
@@ -2017,38 +2083,60 @@
           <t>Audio5</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>123.6711170137764</v>
-      </c>
-      <c r="C6" t="n">
-        <v>113.5146684397178</v>
-      </c>
-      <c r="D6" t="n">
-        <v>110.5522762359554</v>
-      </c>
-      <c r="E6" t="n">
-        <v>108.8243270561412</v>
-      </c>
-      <c r="F6" t="n">
-        <v>107.5248673913698</v>
-      </c>
-      <c r="G6" t="n">
-        <v>106.5759151470831</v>
-      </c>
-      <c r="H6" t="n">
-        <v>105.7630182856831</v>
-      </c>
-      <c r="I6" t="n">
-        <v>105.1132700792296</v>
-      </c>
-      <c r="J6" t="n">
-        <v>104.5662069980139</v>
-      </c>
-      <c r="K6" t="n">
-        <v>104.1908374846282</v>
-      </c>
-      <c r="L6" t="n">
-        <v>104.4450959893519</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>infinite</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -2061,7 +2149,7 @@
         <v>123.6711170137764</v>
       </c>
       <c r="C7" t="n">
-        <v>113.5146684397178</v>
+        <v>113.5120938255811</v>
       </c>
       <c r="D7" t="n">
         <v>110.5522762359554</v>
@@ -2079,16 +2167,16 @@
         <v>105.7630182856831</v>
       </c>
       <c r="I7" t="n">
-        <v>105.1132700792296</v>
+        <v>105.1141384821099</v>
       </c>
       <c r="J7" t="n">
         <v>104.5755128817973</v>
       </c>
       <c r="K7" t="n">
-        <v>104.1406732838857</v>
+        <v>104.1431528980002</v>
       </c>
       <c r="L7" t="n">
-        <v>104.0833443977933</v>
+        <v>104.0884358904425</v>
       </c>
     </row>
     <row r="8">
@@ -2101,7 +2189,7 @@
         <v>123.6445003125738</v>
       </c>
       <c r="C8" t="n">
-        <v>113.5146684397178</v>
+        <v>113.5120938255811</v>
       </c>
       <c r="D8" t="n">
         <v>110.5522762359554</v>
@@ -2122,13 +2210,13 @@
         <v>105.1132700792296</v>
       </c>
       <c r="J8" t="n">
-        <v>104.6784300310068</v>
+        <v>104.6752888225899</v>
       </c>
       <c r="K8" t="n">
-        <v>104.1514947867078</v>
+        <v>104.1497058897571</v>
       </c>
       <c r="L8" t="n">
-        <v>103.9979778309056</v>
+        <v>104.0024898820314</v>
       </c>
     </row>
     <row r="9">
@@ -2165,10 +2253,10 @@
         <v>104.5662069980139</v>
       </c>
       <c r="K9" t="n">
-        <v>104.1334409027093</v>
+        <v>104.1282964050785</v>
       </c>
       <c r="L9" t="n">
-        <v>104.0796274628114</v>
+        <v>104.0815833478313</v>
       </c>
     </row>
     <row r="10">
@@ -2190,25 +2278,25 @@
         <v>108.8243270561412</v>
       </c>
       <c r="F10" t="n">
-        <v>107.5248673913698</v>
+        <v>107.5242190132325</v>
       </c>
       <c r="G10" t="n">
-        <v>106.5759151470831</v>
+        <v>54.22582387954586</v>
       </c>
       <c r="H10" t="n">
-        <v>54.22581867593635</v>
+        <v>105.7625861160349</v>
       </c>
       <c r="I10" t="n">
-        <v>54.22581375647839</v>
+        <v>105.1132700792296</v>
       </c>
       <c r="J10" t="n">
-        <v>104.565878919085</v>
+        <v>104.5655508649383</v>
       </c>
       <c r="K10" t="n">
-        <v>104.0320780940659</v>
+        <v>54.22580372343052</v>
       </c>
       <c r="L10" t="n">
-        <v>103.7258360930134</v>
+        <v>54.22580040369201</v>
       </c>
     </row>
     <row r="11">
@@ -2248,7 +2336,7 @@
         <v>104.0135498150239</v>
       </c>
       <c r="L11" t="n">
-        <v>103.7684018936764</v>
+        <v>103.7706777601298</v>
       </c>
     </row>
     <row r="12">
@@ -2279,16 +2367,16 @@
         <v>105.7625861160349</v>
       </c>
       <c r="I12" t="n">
-        <v>105.1516450313909</v>
+        <v>105.1128979597161</v>
       </c>
       <c r="J12" t="n">
-        <v>105.0058226714146</v>
+        <v>104.5662069980139</v>
       </c>
       <c r="K12" t="n">
-        <v>104.4601181496185</v>
+        <v>104.4530800309526</v>
       </c>
       <c r="L12" t="n">
-        <v>104.9105483860664</v>
+        <v>104.9165903741863</v>
       </c>
     </row>
     <row r="13">
@@ -2325,10 +2413,10 @@
         <v>104.5662069980139</v>
       </c>
       <c r="K13" t="n">
-        <v>104.0321748027408</v>
+        <v>104.0323682265515</v>
       </c>
       <c r="L13" t="n">
-        <v>103.7153044635439</v>
+        <v>103.7169230528485</v>
       </c>
     </row>
     <row r="14">
@@ -2359,16 +2447,16 @@
         <v>105.7630182856831</v>
       </c>
       <c r="I14" t="n">
-        <v>105.2318488480687</v>
+        <v>105.1214647857051</v>
       </c>
       <c r="J14" t="n">
-        <v>104.8052852394682</v>
+        <v>104.8055163516636</v>
       </c>
       <c r="K14" t="n">
-        <v>104.7782148221939</v>
+        <v>104.7623964351688</v>
       </c>
       <c r="L14" t="n">
-        <v>104.4201739514976</v>
+        <v>104.402655244812</v>
       </c>
     </row>
     <row r="15">
@@ -2408,7 +2496,7 @@
         <v>104.0135498150239</v>
       </c>
       <c r="L15" t="n">
-        <v>103.6484824333124</v>
+        <v>103.6450310510904</v>
       </c>
     </row>
     <row r="16">
@@ -2445,10 +2533,10 @@
         <v>104.5662069980139</v>
       </c>
       <c r="K16" t="n">
-        <v>104.033819179787</v>
+        <v>104.0109506038429</v>
       </c>
       <c r="L16" t="n">
-        <v>103.6980769419816</v>
+        <v>103.6960178044372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>